<commit_message>
data provider w tescie, dane z excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin Najwer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin Najwer\Desktop\Tester\Java\Travels\travels\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287353F8-F857-484C-B6CD-B03935FBCD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D383DE71-15F1-4A31-A757-D8BE82759B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="6885" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="4395" windowWidth="21525" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>city</t>
   </si>
@@ -36,10 +36,13 @@
     <t>Dubai</t>
   </si>
   <si>
-    <t>xxx</t>
-  </si>
-  <si>
     <t>London</t>
+  </si>
+  <si>
+    <t>Jumeirah Beach Hotel</t>
+  </si>
+  <si>
+    <t>Grand Plaza Apartments</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,15 +384,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>